<commit_message>
calculated annual removals for co corn
</commit_message>
<xml_diff>
--- a/Old Data/2022 ARDEC 2200 Nutrient Runoff Master List.xlsx
+++ b/Old Data/2022 ARDEC 2200 Nutrient Runoff Master List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\pollinator-strip-runoff\Confidential Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\pollinator-strip-runoff\Old Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70B45AD3-0B04-4E25-82AE-7212DB096688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25AF91C-C034-4537-ADA1-FBD6B7C09929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key For Labeling" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="248">
   <si>
     <t>Site</t>
   </si>
@@ -780,6 +780,9 @@
   </si>
   <si>
     <t>Irr 6</t>
+  </si>
+  <si>
+    <t>sample insufficient for TSS</t>
   </si>
 </sst>
 </file>
@@ -1236,17 +1239,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.265625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1328125" style="1"/>
+    <col min="4" max="4" width="24.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" style="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1280,7 +1283,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1340,7 +1343,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1360,7 +1363,7 @@
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1396,7 +1399,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1410,7 +1413,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1543,20 +1546,20 @@
       <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="8"/>
-    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="8"/>
+    <col min="3" max="3" width="9.73046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="6.7109375" style="8" customWidth="1"/>
+    <col min="6" max="7" width="9.1328125" style="8"/>
+    <col min="8" max="8" width="6.73046875" style="8" customWidth="1"/>
     <col min="9" max="9" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
+    <col min="10" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>54</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>63</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>67</v>
       </c>
@@ -1631,7 +1634,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>72</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>74</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>77</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>78</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>79</v>
       </c>
@@ -1769,7 +1772,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>80</v>
       </c>
@@ -1792,7 +1795,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>81</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>82</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>83</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>84</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>85</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>86</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>87</v>
       </c>
@@ -1953,7 +1956,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
         <v>88</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>89</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>90</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>91</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>92</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>93</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
         <v>94</v>
       </c>
@@ -2114,7 +2117,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
         <v>95</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="8" t="s">
         <v>96</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="8" t="s">
         <v>97</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>98</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
         <v>99</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>100</v>
       </c>
@@ -2252,7 +2255,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>101</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>102</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="8" t="s">
         <v>103</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>104</v>
       </c>
@@ -2344,7 +2347,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>105</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
         <v>106</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
         <v>107</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="8" t="s">
         <v>108</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
         <v>109</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="8" t="s">
         <v>110</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="8" t="s">
         <v>111</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
         <v>112</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
         <v>113</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>114</v>
       </c>
@@ -2574,7 +2577,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>115</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
         <v>116</v>
       </c>
@@ -2620,7 +2623,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>117</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>118</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="8" t="s">
         <v>119</v>
       </c>
@@ -2689,7 +2692,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="8" t="s">
         <v>120</v>
       </c>
@@ -2712,7 +2715,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
         <v>121</v>
       </c>
@@ -2735,7 +2738,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="8" t="s">
         <v>122</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="8" t="s">
         <v>123</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>124</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>125</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="8" t="s">
         <v>126</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="8" t="s">
         <v>127</v>
       </c>
@@ -2873,7 +2876,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="8" t="s">
         <v>128</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>129</v>
       </c>
@@ -2919,7 +2922,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>130</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="8" t="s">
         <v>131</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="8" t="s">
         <v>132</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>133</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="8" t="s">
         <v>134</v>
       </c>
@@ -3034,7 +3037,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="8" t="s">
         <v>135</v>
       </c>
@@ -3057,7 +3060,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="8" t="s">
         <v>136</v>
       </c>
@@ -3080,7 +3083,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="8" t="s">
         <v>137</v>
       </c>
@@ -3103,7 +3106,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="8" t="s">
         <v>138</v>
       </c>
@@ -3126,7 +3129,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="8" t="s">
         <v>139</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="8" t="s">
         <v>140</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="8" t="s">
         <v>141</v>
       </c>
@@ -3195,7 +3198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="8" t="s">
         <v>142</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="8" t="s">
         <v>143</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="8" t="s">
         <v>144</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="8" t="s">
         <v>145</v>
       </c>
@@ -3287,7 +3290,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="8" t="s">
         <v>146</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
         <v>147</v>
       </c>
@@ -3333,7 +3336,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="8" t="s">
         <v>148</v>
       </c>
@@ -3356,7 +3359,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="8" t="s">
         <v>149</v>
       </c>
@@ -3379,7 +3382,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="8" t="s">
         <v>150</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="8" t="s">
         <v>151</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="8" t="s">
         <v>152</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="8" t="s">
         <v>153</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="8" t="s">
         <v>154</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="8" t="s">
         <v>155</v>
       </c>
@@ -3517,7 +3520,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="8" t="s">
         <v>156</v>
       </c>
@@ -3540,7 +3543,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="8" t="s">
         <v>157</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="8" t="s">
         <v>158</v>
       </c>
@@ -3586,7 +3589,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="8" t="s">
         <v>159</v>
       </c>
@@ -3609,7 +3612,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="8" t="s">
         <v>160</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="8" t="s">
         <v>161</v>
       </c>
@@ -3655,7 +3658,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="8" t="s">
         <v>162</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="8" t="s">
         <v>163</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="8" t="s">
         <v>164</v>
       </c>
@@ -3724,7 +3727,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="8" t="s">
         <v>165</v>
       </c>
@@ -3747,7 +3750,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="8" t="s">
         <v>166</v>
       </c>
@@ -3770,7 +3773,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="8" t="s">
         <v>167</v>
       </c>
@@ -3793,7 +3796,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="8" t="s">
         <v>168</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="8" t="s">
         <v>169</v>
       </c>
@@ -3839,7 +3842,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="8" t="s">
         <v>170</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="8" t="s">
         <v>171</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" s="8" t="s">
         <v>172</v>
       </c>
@@ -3908,7 +3911,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" s="8" t="s">
         <v>173</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="8" t="s">
         <v>174</v>
       </c>
@@ -3954,7 +3957,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" s="8" t="s">
         <v>175</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="8" t="s">
         <v>176</v>
       </c>
@@ -4000,7 +4003,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" s="8" t="s">
         <v>177</v>
       </c>
@@ -4023,7 +4026,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" s="8" t="s">
         <v>178</v>
       </c>
@@ -4046,7 +4049,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="8" t="s">
         <v>179</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" s="8" t="s">
         <v>180</v>
       </c>
@@ -4092,7 +4095,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" s="8" t="s">
         <v>181</v>
       </c>
@@ -4115,7 +4118,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114" s="8" t="s">
         <v>182</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115" s="8" t="s">
         <v>183</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A116" s="8" t="s">
         <v>184</v>
       </c>
@@ -4184,7 +4187,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A117" s="8" t="s">
         <v>185</v>
       </c>
@@ -4207,7 +4210,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A118" s="8" t="s">
         <v>186</v>
       </c>
@@ -4230,7 +4233,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A119" s="8" t="s">
         <v>187</v>
       </c>
@@ -4253,7 +4256,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A120" s="8" t="s">
         <v>188</v>
       </c>
@@ -4276,7 +4279,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A121" s="8" t="s">
         <v>189</v>
       </c>
@@ -4299,7 +4302,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A122" s="8" t="s">
         <v>190</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A123" s="8" t="s">
         <v>191</v>
       </c>
@@ -4345,7 +4348,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A124" s="8" t="s">
         <v>192</v>
       </c>
@@ -4368,7 +4371,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A125" s="8" t="s">
         <v>193</v>
       </c>
@@ -4391,7 +4394,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A126" s="8" t="s">
         <v>194</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A127" s="8" t="s">
         <v>195</v>
       </c>
@@ -4437,7 +4440,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A128" s="8" t="s">
         <v>196</v>
       </c>
@@ -4475,18 +4478,18 @@
       <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -4512,7 +4515,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>63</v>
       </c>
@@ -4536,7 +4539,7 @@
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>67</v>
       </c>
@@ -4560,7 +4563,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
@@ -4584,7 +4587,7 @@
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>74</v>
       </c>
@@ -4608,7 +4611,7 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>77</v>
       </c>
@@ -4632,7 +4635,7 @@
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>78</v>
       </c>
@@ -4656,7 +4659,7 @@
       </c>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>79</v>
       </c>
@@ -4680,7 +4683,7 @@
       </c>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>81</v>
       </c>
@@ -4704,7 +4707,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
@@ -4728,7 +4731,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>83</v>
       </c>
@@ -4752,7 +4755,7 @@
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>84</v>
       </c>
@@ -4776,7 +4779,7 @@
       </c>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>86</v>
       </c>
@@ -4800,7 +4803,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>87</v>
       </c>
@@ -4824,7 +4827,7 @@
       </c>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>88</v>
       </c>
@@ -4847,7 +4850,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>89</v>
       </c>
@@ -4872,7 +4875,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>91</v>
       </c>
@@ -4897,7 +4900,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -4922,7 +4925,7 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>92</v>
       </c>
@@ -4947,7 +4950,7 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>93</v>
       </c>
@@ -4972,7 +4975,7 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>94</v>
       </c>
@@ -4997,7 +5000,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>96</v>
       </c>
@@ -5022,7 +5025,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>97</v>
       </c>
@@ -5047,7 +5050,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
         <v>98</v>
       </c>
@@ -5072,7 +5075,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
         <v>99</v>
       </c>
@@ -5097,7 +5100,7 @@
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="8" t="s">
         <v>101</v>
       </c>
@@ -5122,7 +5125,7 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="8" t="s">
         <v>102</v>
       </c>
@@ -5147,7 +5150,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>103</v>
       </c>
@@ -5172,7 +5175,7 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
         <v>104</v>
       </c>
@@ -5196,7 +5199,7 @@
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>106</v>
       </c>
@@ -5220,7 +5223,7 @@
       </c>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>107</v>
       </c>
@@ -5244,7 +5247,7 @@
       </c>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>108</v>
       </c>
@@ -5268,7 +5271,7 @@
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="8" t="s">
         <v>109</v>
       </c>
@@ -5292,7 +5295,7 @@
       </c>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>111</v>
       </c>
@@ -5316,7 +5319,7 @@
       </c>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
@@ -5340,7 +5343,7 @@
       </c>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
         <v>112</v>
       </c>
@@ -5364,7 +5367,7 @@
       </c>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
         <v>113</v>
       </c>
@@ -5388,7 +5391,7 @@
       </c>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="8" t="s">
         <v>114</v>
       </c>
@@ -5412,7 +5415,7 @@
       </c>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
         <v>116</v>
       </c>
@@ -5436,7 +5439,7 @@
       </c>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="8" t="s">
         <v>117</v>
       </c>
@@ -5460,7 +5463,7 @@
       </c>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="8" t="s">
         <v>118</v>
       </c>
@@ -5484,7 +5487,7 @@
       </c>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
         <v>119</v>
       </c>
@@ -5508,7 +5511,7 @@
       </c>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
         <v>121</v>
       </c>
@@ -5532,7 +5535,7 @@
       </c>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>122</v>
       </c>
@@ -5556,7 +5559,7 @@
       </c>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>123</v>
       </c>
@@ -5580,7 +5583,7 @@
       </c>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
         <v>124</v>
       </c>
@@ -5604,7 +5607,7 @@
       </c>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>126</v>
       </c>
@@ -5628,7 +5631,7 @@
       </c>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>127</v>
       </c>
@@ -5652,7 +5655,7 @@
       </c>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="8" t="s">
         <v>128</v>
       </c>
@@ -5676,7 +5679,7 @@
       </c>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="8" t="s">
         <v>129</v>
       </c>
@@ -5700,7 +5703,7 @@
       </c>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
         <v>131</v>
       </c>
@@ -5724,7 +5727,7 @@
       </c>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
@@ -5747,7 +5750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="8" t="s">
         <v>132</v>
       </c>
@@ -5770,7 +5773,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>133</v>
       </c>
@@ -5793,7 +5796,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>134</v>
       </c>
@@ -5816,7 +5819,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="8" t="s">
         <v>136</v>
       </c>
@@ -5840,7 +5843,7 @@
       </c>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="8" t="s">
         <v>137</v>
       </c>
@@ -5864,7 +5867,7 @@
       </c>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="8" t="s">
         <v>138</v>
       </c>
@@ -5888,7 +5891,7 @@
       </c>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>139</v>
       </c>
@@ -5912,7 +5915,7 @@
       </c>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>141</v>
       </c>
@@ -5936,7 +5939,7 @@
       </c>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="8" t="s">
         <v>142</v>
       </c>
@@ -5960,7 +5963,7 @@
       </c>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="8" t="s">
         <v>143</v>
       </c>
@@ -5984,7 +5987,7 @@
       </c>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>144</v>
       </c>
@@ -6008,7 +6011,7 @@
       </c>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="8" t="s">
         <v>146</v>
       </c>
@@ -6032,7 +6035,7 @@
       </c>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>54</v>
       </c>
@@ -6056,7 +6059,7 @@
       </c>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="8" t="s">
         <v>152</v>
       </c>
@@ -6080,7 +6083,7 @@
       </c>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="8" t="s">
         <v>153</v>
       </c>
@@ -6104,7 +6107,7 @@
       </c>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="8" t="s">
         <v>154</v>
       </c>
@@ -6128,7 +6131,7 @@
       </c>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="8" t="s">
         <v>156</v>
       </c>
@@ -6151,7 +6154,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="8" t="s">
         <v>157</v>
       </c>
@@ -6174,7 +6177,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="8" t="s">
         <v>158</v>
       </c>
@@ -6197,7 +6200,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="8" t="s">
         <v>159</v>
       </c>
@@ -6220,7 +6223,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="8" t="s">
         <v>161</v>
       </c>
@@ -6243,7 +6246,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="8" t="s">
         <v>162</v>
       </c>
@@ -6266,7 +6269,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="8" t="s">
         <v>163</v>
       </c>
@@ -6289,7 +6292,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="8" t="s">
         <v>164</v>
       </c>
@@ -6312,7 +6315,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
         <v>166</v>
       </c>
@@ -6335,7 +6338,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="8" t="s">
         <v>167</v>
       </c>
@@ -6358,7 +6361,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="8" t="s">
         <v>168</v>
       </c>
@@ -6381,7 +6384,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" s="8" t="s">
         <v>169</v>
       </c>
@@ -6404,7 +6407,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="8" t="s">
         <v>171</v>
       </c>
@@ -6427,7 +6430,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>54</v>
       </c>
@@ -6450,7 +6453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="8" t="s">
         <v>172</v>
       </c>
@@ -6473,7 +6476,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="8" t="s">
         <v>173</v>
       </c>
@@ -6496,7 +6499,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="8" t="s">
         <v>174</v>
       </c>
@@ -6519,7 +6522,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="8" t="s">
         <v>176</v>
       </c>
@@ -6542,7 +6545,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="8" t="s">
         <v>177</v>
       </c>
@@ -6565,7 +6568,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="8" t="s">
         <v>178</v>
       </c>
@@ -6588,7 +6591,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="8" t="s">
         <v>179</v>
       </c>
@@ -6611,7 +6614,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="8" t="s">
         <v>181</v>
       </c>
@@ -6634,7 +6637,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="8" t="s">
         <v>182</v>
       </c>
@@ -6657,7 +6660,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="8" t="s">
         <v>183</v>
       </c>
@@ -6680,7 +6683,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="8" t="s">
         <v>184</v>
       </c>
@@ -6703,7 +6706,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="8" t="s">
         <v>186</v>
       </c>
@@ -6726,7 +6729,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="8" t="s">
         <v>187</v>
       </c>
@@ -6749,7 +6752,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="8" t="s">
         <v>188</v>
       </c>
@@ -6772,7 +6775,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="8" t="s">
         <v>189</v>
       </c>
@@ -6795,7 +6798,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="8" t="s">
         <v>191</v>
       </c>
@@ -6818,7 +6821,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="8" t="s">
         <v>192</v>
       </c>
@@ -6841,7 +6844,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="8" t="s">
         <v>193</v>
       </c>
@@ -6864,7 +6867,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="8" t="s">
         <v>194</v>
       </c>
@@ -6887,7 +6890,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="8" t="s">
         <v>196</v>
       </c>
@@ -6922,19 +6925,19 @@
   <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="12"/>
+    <col min="1" max="1" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.1328125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6970,7 +6973,7 @@
       <c r="W1" s="21"/>
       <c r="X1" s="21"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>202</v>
       </c>
@@ -7047,7 +7050,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2200</v>
       </c>
@@ -7085,7 +7088,7 @@
         <v>216.66666666666501</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2200</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>36.666666666670032</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2200</v>
       </c>
@@ -7161,7 +7164,7 @@
         <v>903.33333333333746</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2200</v>
       </c>
@@ -7199,7 +7202,7 @@
         <v>930.00000000000114</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2200</v>
       </c>
@@ -7237,7 +7240,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2200</v>
       </c>
@@ -7276,7 +7279,7 @@
       </c>
       <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2200</v>
       </c>
@@ -7318,7 +7321,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2200</v>
       </c>
@@ -7356,7 +7359,7 @@
         <v>103.33329999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2200</v>
       </c>
@@ -7394,7 +7397,7 @@
         <v>363.33330000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2200</v>
       </c>
@@ -7432,7 +7435,7 @@
         <v>353.33330000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2200</v>
       </c>
@@ -7473,7 +7476,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2200</v>
       </c>
@@ -7511,7 +7514,7 @@
         <v>56.666670000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2200</v>
       </c>
@@ -7549,7 +7552,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2200</v>
       </c>
@@ -7587,7 +7590,7 @@
         <v>36.67</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>2200</v>
       </c>
@@ -7625,7 +7628,7 @@
         <v>36.67</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>2200</v>
       </c>
@@ -7659,8 +7662,11 @@
       <c r="L18" s="19">
         <v>8.0999999999999996E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>2200</v>
       </c>
@@ -7694,8 +7700,11 @@
       <c r="L19" s="19">
         <v>9.4999999999999998E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>2200</v>
       </c>
@@ -7729,8 +7738,11 @@
       <c r="L20" s="19">
         <v>8.3000000000000001E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2200</v>
       </c>
@@ -7764,8 +7776,11 @@
       <c r="L21" s="19">
         <v>8.8999999999999999E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2200</v>
       </c>
@@ -7799,8 +7814,11 @@
       <c r="L22" s="19">
         <v>8.6499999999999997E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2200</v>
       </c>
@@ -7834,8 +7852,11 @@
       <c r="L23" s="19">
         <v>9.5399999999999999E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2200</v>
       </c>
@@ -7869,8 +7890,11 @@
       <c r="L24" s="19">
         <v>9.3399999999999993E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y24" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2200</v>
       </c>
@@ -7904,8 +7928,11 @@
       <c r="L25" s="19">
         <v>8.2299999999999995E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>2200</v>
       </c>
@@ -7938,6 +7965,9 @@
       </c>
       <c r="L26" s="19">
         <v>8.3099999999999997E-3</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -7953,26 +7983,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678F2DA36292A241BB6B602A04ACAAD9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d9fb0f190deb5e7e937e6d8ad317d77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="167cb1e9-24b5-43e0-9f5d-14a54474cc90" xmlns:ns3="fbf6f0f6-9634-473c-8838-2f74fc79f714" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="211896cd03a7fb44aac70cae515804dc" ns2:_="" ns3:_="">
     <xsd:import namespace="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
@@ -8221,26 +8231,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1AE484-63F9-47BD-8139-BE7672B2F6CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
-    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54D3016-F8BA-4E9E-81BD-16C0766BD92C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{966B5863-F22D-4BEF-9FEC-9DA16E4E9FE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8257,4 +8268,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54D3016-F8BA-4E9E-81BD-16C0766BD92C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1AE484-63F9-47BD-8139-BE7672B2F6CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>